<commit_message>
Did some more testing and finished section on report about the Blur kernel (minus the conclusion).
</commit_message>
<xml_diff>
--- a/Times.xlsx
+++ b/Times.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6045" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Lena - Blur radius 1-15" sheetId="1" r:id="rId1"/>
+    <sheet name="Lena - Blur radius 1-15 - CPU" sheetId="1" r:id="rId1"/>
+    <sheet name="Lena - Blur radius 1-15 - GPU" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>Blur Radius</t>
   </si>
@@ -109,7 +111,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Lena - Blur radius 1-15'!$B$1</c:f>
+              <c:f>'Lena - Blur radius 1-15 - CPU'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -132,7 +134,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Lena - Blur radius 1-15'!$A$2:$A$16</c:f>
+              <c:f>'Lena - Blur radius 1-15 - CPU'!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -186,7 +188,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Lena - Blur radius 1-15'!$B$2:$B$16</c:f>
+              <c:f>'Lena - Blur radius 1-15 - CPU'!$B$2:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -521,7 +523,484 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Lena - Blur radius 1-15 - GPU'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Lena - Blur radius 1-15 - GPU'!$A$2:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Lena - Blur radius 1-15 - GPU'!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.45992E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6867699999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4389199999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.8969199999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11994299999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.158416</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.233708</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.29578100000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33590999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.39696999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.49583199999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.57770999999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.67206699999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.75311700000000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.897818</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C08F-43F2-84FA-192BFABCDD73}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="484175440"/>
+        <c:axId val="484175768"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="484175440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Blur Radius</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="484175768"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="484175768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="484175440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1077,6 +1556,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1095,6 +2090,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>552449</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1377,8 +2407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1518,4 +2548,151 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1.45992E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>4.6867699999999998E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>4.4389199999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>6.8969199999999994E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.11994299999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.158416</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.233708</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.29578100000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.33590999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0.39696999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0.49583199999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0.57770999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0.67206699999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0.75311700000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0.897818</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added a kernel for adding the blurred image to the original and recorded times for it.
</commit_message>
<xml_diff>
--- a/Times.xlsx
+++ b/Times.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6045" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6045" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lena - Blur radius 1-15 - CPU" sheetId="1" r:id="rId1"/>
     <sheet name="Lena - Blur radius 1-15 - GPU" sheetId="2" r:id="rId2"/>
+    <sheet name="Lena - Blur radius 1-15 - GPU 2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
   <si>
     <t>Blur Radius</t>
   </si>
@@ -292,7 +292,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -413,7 +412,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -960,6 +958,443 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Lena - Blur radius 1-15 - GPU 2'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Lena - Blur radius 1-15 - GPU 2'!$A$2:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Lena - Blur radius 1-15 - GPU 2'!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>8.7630999999999994E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2539999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8678799999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.4445300000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.10494199999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.18723500000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23094100000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.27776000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33649099999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.40751799999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.50319400000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55664999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.68238600000000005</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.80017400000000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.88928399999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1EEE-423B-9B73-318B0670949E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="501209184"/>
+        <c:axId val="501210496"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="501209184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Radius</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="501210496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="501210496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="501209184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1040,6 +1475,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1557,6 +2032,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2121,6 +3112,41 @@
       <xdr:colOff>428624</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2554,8 +3580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2695,4 +3721,151 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>8.7630999999999994E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3.2539999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3.8678799999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>8.4445300000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.10494199999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.18723500000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.23094100000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.27776000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.33649099999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0.40751799999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0.50319400000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0.55664999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0.68238600000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0.80017400000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0.88928399999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ran tests and added tests for ghost-town image.
</commit_message>
<xml_diff>
--- a/Times.xlsx
+++ b/Times.xlsx
@@ -2,21 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Floofy\Projects\unsharp-mask\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unsharp-mask\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6045" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6045" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Lena - Blur radius 1-15 - CPU" sheetId="1" r:id="rId1"/>
     <sheet name="Lena - Blur radius 1-15 - GPU" sheetId="2" r:id="rId2"/>
     <sheet name="Lena - Blur radius 1-15 - GPU 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Ghost - Blur radius 1-15 - CPU" sheetId="4" r:id="rId4"/>
+    <sheet name="Ghost - Blur radius 1-15 - GPU" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="2">
   <si>
     <t>Blur Radius</t>
   </si>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -87,7 +89,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -241,7 +243,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F5BF-4AE9-A89D-056B7DE81B7A}"/>
             </c:ext>
@@ -256,446 +258,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="481213528"/>
-        <c:axId val="481004192"/>
+        <c:axId val="193074088"/>
+        <c:axId val="192778904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="481213528"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Blur Radius</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="481004192"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="481004192"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Time</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="481213528"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Lena - Blur radius 1-15 - GPU'!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Lena - Blur radius 1-15 - GPU'!$A$2:$A$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Lena - Blur radius 1-15 - GPU'!$B$2:$B$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>1.45992E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.6867699999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.4389199999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.8969199999999994E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.11994299999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.158416</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.233708</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.29578100000000002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.33590999999999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.39696999999999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.49583199999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.57770999999999995</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.67206699999999997</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.75311700000000004</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.897818</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C08F-43F2-84FA-192BFABCDD73}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="484175440"/>
-        <c:axId val="484175768"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="484175440"/>
+        <c:axId val="193074088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -794,7 +361,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="484175768"/>
+        <c:crossAx val="192778904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -802,7 +369,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="484175768"/>
+        <c:axId val="192778904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -909,7 +476,442 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="484175440"/>
+        <c:crossAx val="193074088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Lena - Blur radius 1-15 - GPU'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Lena - Blur radius 1-15 - GPU'!$A$2:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Lena - Blur radius 1-15 - GPU'!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.45992E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6867699999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4389199999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.8969199999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11994299999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.158416</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.233708</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.29578100000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33590999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.39696999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.49583199999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.57770999999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.67206699999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.75311700000000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.897818</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C08F-43F2-84FA-192BFABCDD73}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="193062760"/>
+        <c:axId val="193232440"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="193062760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Blur Radius</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="193232440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="193232440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="193062760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -959,7 +961,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1113,7 +1115,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1EEE-423B-9B73-318B0670949E}"/>
             </c:ext>
@@ -1128,11 +1130,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="501209184"/>
-        <c:axId val="501210496"/>
+        <c:axId val="193281360"/>
+        <c:axId val="193316336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="501209184"/>
+        <c:axId val="193281360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,7 +1233,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="501210496"/>
+        <c:crossAx val="193316336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1239,7 +1241,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="501210496"/>
+        <c:axId val="193316336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1346,7 +1348,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="501209184"/>
+        <c:crossAx val="193281360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3727,7 +3729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
@@ -3868,4 +3870,296 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>9.0715199999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>10.733700000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>13.929600000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>18.677099999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>24.765699999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>32.523499999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>41.867100000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>52.557899999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>65.093500000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>78.935599999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>97.812299999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>115.33499999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>132.98599999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>158.85900000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>180.99600000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3.8933500000000003E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>6.3576099999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.107596</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.176098</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.268181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.38212299999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.52070499999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.68252199999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.86475800000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1.07403</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1.2976700000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1.53633</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1.8124899999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>2.1150899999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>2.4420999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>